<commit_message>
Fix a bug where cells with empty text weren't explicitely written to file.
That caused several issues, including invalid files, because SST wrote -1 as a SST index.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFIsBlank.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/ConditionalFormatting/CFIsBlank.xlsx
@@ -17,6 +17,9 @@
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Hello</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
   </x:si>
   <x:si>
     <x:t>Holl</x:t>
@@ -391,9 +394,14 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:1">
+      <x:c r="A3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
     <x:row r="4" spans="1:1">
       <x:c r="A4" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>